<commit_message>
Fix 4034 4044 and 4045 samples
</commit_message>
<xml_diff>
--- a/RNASeq_scripts/dataKentaro/samples concentration.xlsx
+++ b/RNASeq_scripts/dataKentaro/samples concentration.xlsx
@@ -312,7 +312,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -624,11 +624,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="56912773"/>
-        <c:axId val="84016304"/>
+        <c:axId val="83879348"/>
+        <c:axId val="44469401"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56912773"/>
+        <c:axId val="83879348"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -670,14 +670,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84016304"/>
+        <c:crossAx val="44469401"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84016304"/>
+        <c:axId val="44469401"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +719,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56912773"/>
+        <c:crossAx val="83879348"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -747,7 +747,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1063,11 +1063,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="91320525"/>
-        <c:axId val="99939943"/>
+        <c:axId val="3261018"/>
+        <c:axId val="73333607"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="91320525"/>
+        <c:axId val="3261018"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,14 +1133,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99939943"/>
+        <c:crossAx val="73333607"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99939943"/>
+        <c:axId val="73333607"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1206,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91320525"/>
+        <c:crossAx val="3261018"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1258,7 +1258,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1574,11 +1574,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="37600874"/>
-        <c:axId val="23111960"/>
+        <c:axId val="17132122"/>
+        <c:axId val="99987455"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37600874"/>
+        <c:axId val="17132122"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,14 +1644,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23111960"/>
+        <c:crossAx val="99987455"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23111960"/>
+        <c:axId val="99987455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1717,7 +1717,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37600874"/>
+        <c:crossAx val="17132122"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1769,7 +1769,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1815,10 +1815,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0681157120947697"/>
-          <c:y val="0.162383471907281"/>
-          <c:w val="0.871172457559892"/>
-          <c:h val="0.720836482741245"/>
+          <c:x val="0.0681229174379859"/>
+          <c:y val="0.16242439516129"/>
+          <c:w val="0.871053049135241"/>
+          <c:h val="0.720766129032258"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2050,11 +2050,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="25327889"/>
-        <c:axId val="15874201"/>
+        <c:axId val="19520257"/>
+        <c:axId val="99189911"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25327889"/>
+        <c:axId val="19520257"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2096,12 +2096,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15874201"/>
+        <c:crossAx val="99189911"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15874201"/>
+        <c:axId val="99189911"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2143,7 +2143,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25327889"/>
+        <c:crossAx val="19520257"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2182,9 +2182,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>485640</xdr:colOff>
+      <xdr:colOff>484920</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2193,7 +2193,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12372840" y="346680"/>
-        <a:ext cx="5994360" cy="2856960"/>
+        <a:ext cx="5993640" cy="2856240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2212,9 +2212,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:colOff>132480</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>47160</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2223,7 +2223,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="4559040" y="5457600"/>
-        <a:ext cx="7765920" cy="2781000"/>
+        <a:ext cx="7765200" cy="2780280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2242,9 +2242,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>171000</xdr:colOff>
+      <xdr:colOff>170280</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2253,7 +2253,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12668040" y="5924520"/>
-        <a:ext cx="6197040" cy="2742840"/>
+        <a:ext cx="6196320" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2277,9 +2277,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>594000</xdr:colOff>
+      <xdr:colOff>593280</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2288,7 +2288,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2727720" y="5379480"/>
-        <a:ext cx="6806880" cy="2857320"/>
+        <a:ext cx="6806160" cy="2856600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5136,7 +5136,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5564,7 +5564,7 @@
         <v>198.8</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L10" s="0" t="n">
         <f aca="false">F10/J10</f>
@@ -5653,7 +5653,7 @@
         <v>170.9</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L12" s="0" t="n">
         <f aca="false">F12/J12</f>
@@ -5692,7 +5692,7 @@
         <v>191.7</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L13" s="0" t="n">
         <f aca="false">F13/J13</f>

</xml_diff>